<commit_message>
Mengubah data toko ajat
</commit_message>
<xml_diff>
--- a/CSP-Toko-Ajat/data-fiksi.xlsx
+++ b/CSP-Toko-Ajat/data-fiksi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
   <si>
     <t>Gunung Gelas</t>
   </si>
@@ -105,6 +105,30 @@
   </si>
   <si>
     <t>1 bks</t>
+  </si>
+  <si>
+    <t>harga_jual</t>
+  </si>
+  <si>
+    <t>kategori</t>
+  </si>
+  <si>
+    <t>nama_produk</t>
+  </si>
+  <si>
+    <t>satuan</t>
+  </si>
+  <si>
+    <t>harga_beli</t>
+  </si>
+  <si>
+    <t>kecepatan_penjualan_per_hari</t>
+  </si>
+  <si>
+    <t>jumlah_modal_stok</t>
+  </si>
+  <si>
+    <t>jumlah_stok_sekarang</t>
   </si>
 </sst>
 </file>
@@ -422,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +457,33 @@
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -458,12 +508,8 @@
       <c r="H2">
         <v>9</v>
       </c>
-      <c r="I2">
-        <f>G2-H2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -488,12 +534,8 @@
       <c r="H3">
         <v>4</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I22" si="0">G3-H3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -518,12 +560,8 @@
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -548,12 +586,8 @@
       <c r="H5">
         <v>2</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -578,12 +612,8 @@
       <c r="H6">
         <v>2</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -608,12 +638,8 @@
       <c r="H7">
         <v>4</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -638,12 +664,8 @@
       <c r="H8">
         <v>6</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -668,12 +690,8 @@
       <c r="H9">
         <v>7</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -698,12 +716,8 @@
       <c r="H10">
         <v>6</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -728,12 +742,8 @@
       <c r="H11">
         <v>5</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -758,12 +768,8 @@
       <c r="H12">
         <v>3</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -788,12 +794,8 @@
       <c r="H13">
         <v>4</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -818,12 +820,8 @@
       <c r="H14">
         <v>2</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -848,12 +846,8 @@
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -878,12 +872,8 @@
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -908,12 +898,8 @@
       <c r="H17">
         <v>2</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -938,12 +924,8 @@
       <c r="H18">
         <v>3</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -968,12 +950,8 @@
       <c r="H19">
         <v>3</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -998,12 +976,8 @@
       <c r="H20">
         <v>2</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1028,12 +1002,8 @@
       <c r="H21">
         <v>2</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1057,10 +1027,6 @@
       </c>
       <c r="H22">
         <v>3</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>